<commit_message>
Project Finally Fully Complete
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -1,35 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaur\Documents\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADB797D-C081-4153-B2AF-56C05CDE8ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BB0925-FF85-411B-91B0-94922EFD98AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11775" yWindow="3135" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="1965" windowWidth="15375" windowHeight="7875" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDEX" sheetId="1" r:id="rId1"/>
     <sheet name="VDT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1625030709" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1625030709" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1625030709" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1625030709"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="264">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -586,16 +579,258 @@
   </si>
   <si>
     <t>Bibliography</t>
+  </si>
+  <si>
+    <t>disp</t>
+  </si>
+  <si>
+    <t>ut1</t>
+  </si>
+  <si>
+    <t>ut2</t>
+  </si>
+  <si>
+    <t>ut3</t>
+  </si>
+  <si>
+    <t>ut4</t>
+  </si>
+  <si>
+    <t>ClassTest</t>
+  </si>
+  <si>
+    <t>To store marks of UT 1</t>
+  </si>
+  <si>
+    <t>To store marks of UT 2</t>
+  </si>
+  <si>
+    <t>To store marks of UT 3</t>
+  </si>
+  <si>
+    <t>To store marks of UT 4</t>
+  </si>
+  <si>
+    <t>function to display the marks</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>To store marks th final term</t>
+  </si>
+  <si>
+    <t>FinalExam</t>
+  </si>
+  <si>
+    <t>compute</t>
+  </si>
+  <si>
+    <t>To calculate total marks</t>
+  </si>
+  <si>
+    <t>total_marks</t>
+  </si>
+  <si>
+    <t>To store total marks</t>
+  </si>
+  <si>
+    <t>operate()</t>
+  </si>
+  <si>
+    <t>char[]</t>
+  </si>
+  <si>
+    <t>keyV</t>
+  </si>
+  <si>
+    <t>keyC</t>
+  </si>
+  <si>
+    <t>keyO</t>
+  </si>
+  <si>
+    <t>V_arr</t>
+  </si>
+  <si>
+    <t>C_arr</t>
+  </si>
+  <si>
+    <t>O_arr</t>
+  </si>
+  <si>
+    <t>Vpos</t>
+  </si>
+  <si>
+    <t>Cpos</t>
+  </si>
+  <si>
+    <t>Opos</t>
+  </si>
+  <si>
+    <t>letarr</t>
+  </si>
+  <si>
+    <t>posarr</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>input(int)</t>
+  </si>
+  <si>
+    <t>append(int[], int)</t>
+  </si>
+  <si>
+    <t>generateKey()</t>
+  </si>
+  <si>
+    <t>extractKey()</t>
+  </si>
+  <si>
+    <t>checkArray(char[])</t>
+  </si>
+  <si>
+    <t>intcrement(char[], int)</t>
+  </si>
+  <si>
+    <t>append(char[], char)</t>
+  </si>
+  <si>
+    <t>decrement(char[], int)</t>
+  </si>
+  <si>
+    <t>fillArrs()</t>
+  </si>
+  <si>
+    <t>sortArrs()</t>
+  </si>
+  <si>
+    <t>joinArrs()</t>
+  </si>
+  <si>
+    <t>formStringFromArrs()</t>
+  </si>
+  <si>
+    <t>encrypt()</t>
+  </si>
+  <si>
+    <t>decrypt()</t>
+  </si>
+  <si>
+    <t>display(int)</t>
+  </si>
+  <si>
+    <t>To store key for vowels</t>
+  </si>
+  <si>
+    <t>To store key for consonants</t>
+  </si>
+  <si>
+    <t>To store key for everything else</t>
+  </si>
+  <si>
+    <t>To store length of the string</t>
+  </si>
+  <si>
+    <t>To store the string from user</t>
+  </si>
+  <si>
+    <t>To store the array of vowels</t>
+  </si>
+  <si>
+    <t>To store the array of consonants</t>
+  </si>
+  <si>
+    <t>To store the array of everything else</t>
+  </si>
+  <si>
+    <t>To store the positions of vowels</t>
+  </si>
+  <si>
+    <t>To store the positions of consonants</t>
+  </si>
+  <si>
+    <t>To store the positions of everything else</t>
+  </si>
+  <si>
+    <t>To store all the characters of the string</t>
+  </si>
+  <si>
+    <t>To store all the positions in the string</t>
+  </si>
+  <si>
+    <t>To store the final string</t>
+  </si>
+  <si>
+    <t>To take input according to choice</t>
+  </si>
+  <si>
+    <t>To append an elemennt to an array</t>
+  </si>
+  <si>
+    <t>To append an  element to an array</t>
+  </si>
+  <si>
+    <t>To generate a random key</t>
+  </si>
+  <si>
+    <t>To extract the key from the  string</t>
+  </si>
+  <si>
+    <t>To check if an array is eligible to be encrypted</t>
+  </si>
+  <si>
+    <t>To shift elements  in  an  array to right</t>
+  </si>
+  <si>
+    <t>To shift elements  in  an  array to left</t>
+  </si>
+  <si>
+    <t>To fill all the arrays</t>
+  </si>
+  <si>
+    <t>To join all the arrays</t>
+  </si>
+  <si>
+    <t>To sort the joined arrays</t>
+  </si>
+  <si>
+    <t>To form a string from letarr</t>
+  </si>
+  <si>
+    <t>To encrypt a string</t>
+  </si>
+  <si>
+    <t>To decrypt a string</t>
+  </si>
+  <si>
+    <t>To display according to choice</t>
+  </si>
+  <si>
+    <t>To take input of choice</t>
+  </si>
+  <si>
+    <t>To call display and input of choice</t>
+  </si>
+  <si>
+    <t>To create object and call operate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -643,14 +878,6 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-    <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1625030709" count="1">
-        <pm:charStyle name="Normal" fontId="0" Id="1"/>
-      </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1625030709" count="1">
-        <pm:color name="Color 24" rgb="D8D8D8"/>
-      </pm:colors>
     </ext>
   </extLst>
 </styleSheet>
@@ -721,6 +948,67 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="DataType/ReturnType"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Variable/Method"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{937B3780-B042-4D49-9066-ACCEFD1947E7}" name="Table214" displayName="Table214" ref="BD1:BG7">
+  <autoFilter ref="BD1:BG7" xr:uid="{937B3780-B042-4D49-9066-ACCEFD1947E7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="BD2:BG6">
+    <sortCondition ref="BD1:BD6"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{2CFD218B-8A5A-4A51-9C34-D713446C8D9F}" name="No." totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{4FA50C4C-DB21-4621-A679-F0D4CBFFF94D}" name="DataType/ReturnType"/>
+    <tableColumn id="3" xr3:uid="{BB117322-C492-410A-9EA8-1E9570D112BB}" name="Variable/Method"/>
+    <tableColumn id="4" xr3:uid="{FF181637-255A-4782-9EB6-93F1F13F8566}" name="Description" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E06D6A91-BB4E-4196-9F8D-E7BBC5BAD647}" name="Table21415" displayName="Table21415" ref="BI1:BL4">
+  <autoFilter ref="BI1:BL4" xr:uid="{E06D6A91-BB4E-4196-9F8D-E7BBC5BAD647}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="BI2:BL6">
+    <sortCondition ref="BI1:BI6"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{5CB5F443-8CBD-41D1-83E1-D52B2AAC3FC1}" name="No." totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{6FA00297-99BF-408E-AC68-0CAD15298083}" name="DataType/ReturnType"/>
+    <tableColumn id="3" xr3:uid="{A7058975-A534-4276-8990-12077E3ACEAF}" name="Variable/Method"/>
+    <tableColumn id="4" xr3:uid="{3DF12C8B-B2AC-401F-BE68-63F2574599F0}" name="Description" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{E28B9A35-5EAA-4ED8-B325-26F2714346E2}" name="Table2141516" displayName="Table2141516" ref="BN1:BQ5">
+  <autoFilter ref="BN1:BQ5" xr:uid="{E28B9A35-5EAA-4ED8-B325-26F2714346E2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="BN2:BQ6">
+    <sortCondition ref="BN1:BN6"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D837F842-A076-4E33-99E9-FDD84ED551FE}" name="No." totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{B0A315F5-DE51-413E-8219-990F81054692}" name="DataType/ReturnType"/>
+    <tableColumn id="3" xr3:uid="{834D29F4-993A-4689-8CB5-9CFD27007822}" name="Variable/Method"/>
+    <tableColumn id="4" xr3:uid="{2CBE8184-C8E5-44B3-991D-A60BF53F01D4}" name="Description" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{B4EDA479-52D2-4EDF-A49B-9A685C51D021}" name="Table217" displayName="Table217" ref="BS1:BV33">
+  <autoFilter ref="BS1:BV33" xr:uid="{B4EDA479-52D2-4EDF-A49B-9A685C51D021}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BF1E9669-4E5C-454C-9645-3E27BBED1DC4}" name="No." totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{AD3ED503-0310-45B3-8187-02249FABDC79}" name="DataType/ReturnType"/>
+    <tableColumn id="3" xr3:uid="{09073342-11B2-439A-B608-F8F7BC00B85A}" name="Variable/Method"/>
+    <tableColumn id="4" xr3:uid="{2113A72B-8D07-4438-9889-78CE67D19591}" name="Description" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1128,7 +1416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="160" workbookViewId="0">
       <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
@@ -1409,23 +1697,15 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1625030709" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BB12"/>
+  <dimension ref="A1:BV33"/>
   <sheetViews>
-    <sheetView topLeftCell="AS5" zoomScale="90" workbookViewId="0">
-      <selection activeCell="AY1" sqref="AY1:BB9"/>
+    <sheetView tabSelected="1" topLeftCell="BS21" zoomScale="90" workbookViewId="0">
+      <selection activeCell="BS1" sqref="BS1:BV33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1717,7 @@
     <col min="5" max="16384" width="20.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1570,8 +1850,56 @@
       <c r="BB1" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="BD1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:74" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1704,8 +2032,56 @@
       <c r="BB2" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="BD2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="BI2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="BN2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="BS2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:74" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1838,8 +2214,56 @@
       <c r="BB3" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="BD3" s="2">
+        <v>2</v>
+      </c>
+      <c r="BE3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BF3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="BG3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="BI3" s="2">
+        <v>2</v>
+      </c>
+      <c r="BJ3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="BL3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BN3" s="2">
+        <v>2</v>
+      </c>
+      <c r="BO3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="BQ3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BS3" s="2">
+        <v>2</v>
+      </c>
+      <c r="BT3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU3" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="BV3" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:74" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1972,8 +2396,56 @@
       <c r="BB4" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:54" ht="75" x14ac:dyDescent="0.25">
+      <c r="BD4" s="2">
+        <v>3</v>
+      </c>
+      <c r="BE4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI4" s="2">
+        <v>3</v>
+      </c>
+      <c r="BJ4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BK4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BL4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="BN4" s="2">
+        <v>3</v>
+      </c>
+      <c r="BO4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BP4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BQ4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="BS4" s="2">
+        <v>3</v>
+      </c>
+      <c r="BT4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU4" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="BV4" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:74" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2106,8 +2578,44 @@
       <c r="BB5" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="6" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="BD5" s="2">
+        <v>4</v>
+      </c>
+      <c r="BE5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BF5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="BG5" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="BN5" s="2">
+        <v>4</v>
+      </c>
+      <c r="BO5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BP5" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="BQ5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BS5" s="2">
+        <v>4</v>
+      </c>
+      <c r="BT5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BV5" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:74" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2240,8 +2748,32 @@
       <c r="BB6" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="7" spans="1:54" ht="90" x14ac:dyDescent="0.25">
+      <c r="BD6" s="2">
+        <v>5</v>
+      </c>
+      <c r="BE6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BF6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BS6" s="2">
+        <v>5</v>
+      </c>
+      <c r="BT6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BU6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BV6" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:74" ht="90" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
       <c r="F7" s="2">
         <v>6</v>
@@ -2363,8 +2895,32 @@
       <c r="BB7" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="8" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="BD7" s="2">
+        <v>6</v>
+      </c>
+      <c r="BE7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BF7" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BG7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="BS7" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT7" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BU7" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="BV7" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:74" ht="60" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
       <c r="F8" s="2">
         <v>7</v>
@@ -2474,8 +3030,20 @@
       <c r="BB8" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="9" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="BS8" s="2">
+        <v>7</v>
+      </c>
+      <c r="BT8" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BU8" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="BV8" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:74" ht="45" x14ac:dyDescent="0.25">
       <c r="F9" s="2">
         <v>8</v>
       </c>
@@ -2560,8 +3128,20 @@
       <c r="BB9" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="10" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="BS9" s="2">
+        <v>8</v>
+      </c>
+      <c r="BT9" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BU9" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="BV9" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:74" ht="45" x14ac:dyDescent="0.25">
       <c r="F10" s="2">
         <v>9</v>
       </c>
@@ -2622,8 +3202,20 @@
       <c r="AM10" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="11" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="BS10" s="2">
+        <v>9</v>
+      </c>
+      <c r="BT10" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="BU10" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="BV10" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:74" ht="45" x14ac:dyDescent="0.25">
       <c r="F11" s="2">
         <v>10</v>
       </c>
@@ -2672,8 +3264,20 @@
       <c r="AM11" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="12" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="BS11" s="2">
+        <v>10</v>
+      </c>
+      <c r="BT11" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="BU11" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="BV11" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:74" ht="45" x14ac:dyDescent="0.25">
       <c r="F12" s="2">
         <v>11</v>
       </c>
@@ -2698,11 +3302,318 @@
       <c r="S12" s="2" t="s">
         <v>160</v>
       </c>
+      <c r="BS12" s="2">
+        <v>11</v>
+      </c>
+      <c r="BT12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="BU12" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BV12" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:74" ht="45" x14ac:dyDescent="0.25">
+      <c r="BS13" s="2">
+        <v>12</v>
+      </c>
+      <c r="BT13" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BU13" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="BV13" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS14" s="2">
+        <v>13</v>
+      </c>
+      <c r="BT14" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="BU14" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="BV14" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS15" s="2">
+        <v>14</v>
+      </c>
+      <c r="BT15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BU15" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="BV15" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS16" s="2">
+        <v>15</v>
+      </c>
+      <c r="BT16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU16" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="BV16" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS17" s="2">
+        <v>16</v>
+      </c>
+      <c r="BT17" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BU17" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="BV17" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS18" s="2">
+        <v>17</v>
+      </c>
+      <c r="BT18" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="BU18" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="BV18" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS19" s="2">
+        <v>18</v>
+      </c>
+      <c r="BT19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU19" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="BV19" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS20" s="2">
+        <v>19</v>
+      </c>
+      <c r="BT20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU20" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="BV20" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="71:74" ht="45" x14ac:dyDescent="0.25">
+      <c r="BS21" s="2">
+        <v>20</v>
+      </c>
+      <c r="BT21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="BU21" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="BV21" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS22" s="2">
+        <v>21</v>
+      </c>
+      <c r="BT22" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BU22" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="BV22" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS23" s="2">
+        <v>22</v>
+      </c>
+      <c r="BT23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BU23" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="BV23" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="71:74" x14ac:dyDescent="0.25">
+      <c r="BS24" s="2">
+        <v>23</v>
+      </c>
+      <c r="BT24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU24" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="BV24" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="71:74" x14ac:dyDescent="0.25">
+      <c r="BS25" s="2">
+        <v>24</v>
+      </c>
+      <c r="BT25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU25" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="BV25" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS26" s="2">
+        <v>25</v>
+      </c>
+      <c r="BT26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU26" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="BV26" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS27" s="2">
+        <v>26</v>
+      </c>
+      <c r="BT27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU27" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="BV27" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="71:74" x14ac:dyDescent="0.25">
+      <c r="BS28" s="2">
+        <v>27</v>
+      </c>
+      <c r="BT28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU28" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="BV28" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="71:74" x14ac:dyDescent="0.25">
+      <c r="BS29" s="2">
+        <v>28</v>
+      </c>
+      <c r="BT29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU29" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="BV29" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS30" s="2">
+        <v>29</v>
+      </c>
+      <c r="BT30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU30" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="BV30" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS31" s="2">
+        <v>30</v>
+      </c>
+      <c r="BT31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BV31" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS32" s="2">
+        <v>31</v>
+      </c>
+      <c r="BT32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU32" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV32" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="71:74" ht="30" x14ac:dyDescent="0.25">
+      <c r="BS33" s="2">
+        <v>32</v>
+      </c>
+      <c r="BT33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU33" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BV33" s="2" t="s">
+        <v>263</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0"/>
-  <tableParts count="11">
+  <tableParts count="15">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -2714,14 +3625,10 @@
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
-  <extLst>
-    <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1625030709" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
-        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
-      </pm:sheetPrefs>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>